<commit_message>
updated upload function - button & popup
</commit_message>
<xml_diff>
--- a/data/Historical_Data.xlsx
+++ b/data/Historical_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isawang/Desktop/proj_Apollo/historical_data_visualizer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341CFCA3-6CC5-D04D-8B65-A55C921A19F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2532706-118F-A64F-AA90-6A387D108EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3972,8 +3972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1977"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1945" workbookViewId="0">
-      <selection activeCell="A1978" sqref="A1978:XFD1978"/>
+    <sheetView tabSelected="1" topLeftCell="A1957" workbookViewId="0">
+      <selection activeCell="H1979" sqref="H1979"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
update auto-refresh, button position
</commit_message>
<xml_diff>
--- a/data/Historical_Data.xlsx
+++ b/data/Historical_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isawang/Desktop/proj_Apollo/historical_data_visualizer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2532706-118F-A64F-AA90-6A387D108EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15B4C92-9B5B-844B-89B8-9A6BF5A51978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3972,8 +3972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1977"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1957" workbookViewId="0">
-      <selection activeCell="H1979" sqref="H1979"/>
+    <sheetView tabSelected="1" topLeftCell="A1949" workbookViewId="0">
+      <selection activeCell="A1978" sqref="A1978:XFD1978"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
updated auto-refetch after operations
</commit_message>
<xml_diff>
--- a/data/Historical_Data.xlsx
+++ b/data/Historical_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isawang/Desktop/proj_Apollo/historical_data_visualizer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15B4C92-9B5B-844B-89B8-9A6BF5A51978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9380F9F2-DD94-7043-9109-3C0B2924403C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3972,8 +3972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1977"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1949" workbookViewId="0">
-      <selection activeCell="A1978" sqref="A1978:XFD1978"/>
+    <sheetView tabSelected="1" topLeftCell="A1954" workbookViewId="0">
+      <selection activeCell="E1977" sqref="E1977"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>

</xml_diff>